<commit_message>
started PA2, added buttons and second layout
</commit_message>
<xml_diff>
--- a/class resources/2018 - CS 480 - Whiteboarding Signups.xlsx
+++ b/class resources/2018 - CS 480 - Whiteboarding Signups.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Day</t>
   </si>
@@ -28,6 +28,78 @@
   </si>
   <si>
     <t>NO SCHOOL</t>
+  </si>
+  <si>
+    <t>Jack Kinne</t>
+  </si>
+  <si>
+    <t>Zach Freeman</t>
+  </si>
+  <si>
+    <t>Levi Pole</t>
+  </si>
+  <si>
+    <t>Chase Cullen</t>
+  </si>
+  <si>
+    <t>Sam Alston</t>
+  </si>
+  <si>
+    <t>Lam Ngo</t>
+  </si>
+  <si>
+    <t>Alec Levin</t>
+  </si>
+  <si>
+    <t>Jeremy Walker</t>
+  </si>
+  <si>
+    <t>David Lynch</t>
+  </si>
+  <si>
+    <t>Sam Papavasiliou</t>
+  </si>
+  <si>
+    <t>Angel Ruiz</t>
+  </si>
+  <si>
+    <t>Casey Tran</t>
+  </si>
+  <si>
+    <t>Eric Mott</t>
+  </si>
+  <si>
+    <t>Julian Lucas</t>
+  </si>
+  <si>
+    <t>Chadwick Davis</t>
+  </si>
+  <si>
+    <t>Raymond Ivey</t>
+  </si>
+  <si>
+    <t>Christopher Johnstone</t>
+  </si>
+  <si>
+    <t>Marcellus Parley</t>
+  </si>
+  <si>
+    <t>Jack Witherell</t>
+  </si>
+  <si>
+    <t>Luis Garcia</t>
+  </si>
+  <si>
+    <t>William Dounda</t>
+  </si>
+  <si>
+    <t>Jared Conn</t>
+  </si>
+  <si>
+    <t>Thomas Murphy</t>
+  </si>
+  <si>
+    <t>Jakob Konicke</t>
   </si>
 </sst>
 </file>
@@ -35,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -68,7 +140,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,18 +421,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,170 +441,242 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43129</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43131</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f>A2+7</f>
+        <f t="shared" ref="A4:A28" si="0">A2+7</f>
         <v>43136</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>A3+7</f>
+        <f t="shared" si="0"/>
         <v>43138</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f>A4+7</f>
+        <f t="shared" si="0"/>
         <v>43143</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>A5+7</f>
+        <f t="shared" si="0"/>
         <v>43145</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f>A6+7</f>
+        <f t="shared" si="0"/>
         <v>43150</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f>A7+7</f>
+        <f t="shared" si="0"/>
         <v>43152</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f>A8+7</f>
+        <f t="shared" si="0"/>
         <v>43157</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f>A9+7</f>
+        <f t="shared" si="0"/>
         <v>43159</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f>A10+7</f>
+        <f t="shared" si="0"/>
         <v>43164</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f>A11+7</f>
+        <f t="shared" si="0"/>
         <v>43166</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f>A12+7</f>
+        <f t="shared" si="0"/>
         <v>43171</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f>A13+7</f>
+        <f t="shared" si="0"/>
         <v>43173</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f>A14+7</f>
+        <f t="shared" si="0"/>
         <v>43178</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f>A15+7</f>
+        <f t="shared" si="0"/>
         <v>43180</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f>A16+7</f>
+        <f t="shared" si="0"/>
         <v>43185</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f>A17+7</f>
+        <f t="shared" si="0"/>
         <v>43187</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f>A18+7</f>
+        <f t="shared" si="0"/>
         <v>43192</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f>A19+7</f>
+        <f t="shared" si="0"/>
         <v>43194</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f>A20+7</f>
+        <f t="shared" si="0"/>
         <v>43199</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f>A21+7</f>
+        <f t="shared" si="0"/>
         <v>43201</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f>A22+7</f>
+        <f t="shared" si="0"/>
         <v>43206</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f>A23+7</f>
+        <f t="shared" si="0"/>
         <v>43208</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f>A24+7</f>
+        <f t="shared" si="0"/>
         <v>43213</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f>A25+7</f>
+        <f t="shared" si="0"/>
         <v>43215</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f>A26+7</f>
+        <f t="shared" si="0"/>
         <v>43220</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
   </sheetData>

</xml_diff>